<commit_message>
arreglo de error de servidor. falta arreglar generador de img (eficiencia)
</commit_message>
<xml_diff>
--- a/IA/tablas_generadas/tablita.xlsx
+++ b/IA/tablas_generadas/tablita.xlsx
@@ -436,96 +436,96 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Criterio</t>
+          <t>criterion</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Mercado Libre</t>
+          <t>mercado_libre</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Amazon</t>
+          <t>amazon</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>PedidoYa</t>
+          <t>pedidoya</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Sitio de la Imagen</t>
+          <t>website_from_image</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Conclusión</t>
+          <t>conclusion</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Tipografía</t>
+          <t>Typography</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Utiliza tipografías claras y legibles, como Proxima Nova, para una experiencia de usuario familiar y eficiente, facilitando la lectura en todo el sitio.</t>
+          <t>Utiliza una tipografía Sans-serif clara y legible, como Arial o Open Sans, que asegura una buena experiencia de lectura en todos sus dispositivos.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Emplea la familia de fuentes Amazon Ember, diseñada para una legibilidad óptima y consistente en diversas interfaces y dispositivos.</t>
+          <t>Emplea una tipografía distintiva (Amazon Ember) para mantener consistencia visual, facilitando la identificación de la marca y la lectura de descripciones de productos.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Su tipografía es moderna y fresca, manteniendo la claridad para una fácil comprensión de la información de los restaurantes y pedidos.</t>
+          <t>Su tipografía es moderna y amigable, a menudo usando una fuente redondeada y sencilla para transmitir accesibilidad y rapidez en el servicio de entrega.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Presenta una tipografía sans-serif estándar, legible y limpia, ideal para la visualización de nombres de componentes y datos técnicos.</t>
+          <t>La tipografía es limpia y moderna, principalmente sans-serif, ofreciendo buena legibilidad para nombres de productos y encabezados importantes en la página.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Experimentar con una fuente de encabezado distintiva, sin sacrificar la legibilidad, podría darle más personalidad al sitio.</t>
+          <t>Considerar incorporar variaciones de peso o tamaño para destacar mejor elementos clave sin comprometer la consistencia global del sitio.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Colores</t>
+          <t>Colors</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Predominan los tonos amarillos y naranjas, asociados a la energía y ofertas, complementados con blancos y grises para un diseño limpio.</t>
+          <t>Domina el amarillo vibrante junto con el azul oscuro, creando un contraste energético que llama la atención y resalta ofertas especiales.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Su paleta se basa en el negro, blanco y un distintivo naranja, creando contraste y dirigiendo la atención a elementos clave.</t>
+          <t>Predominan el blanco, negro y un toque de naranja/azul, generando un esquema de colores profesional que facilita la concentración en los productos mostrados.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Combina rojos vibrantes y blancos, transmitiendo inmediatez y apetito, con un diseño visualmente atractivo y reconocible.</t>
+          <t>Se caracteriza por el rojo brillante y el blanco, transmitiendo energía y urgencia, lo cual es muy apropiado para su modelo de negocio de entrega rápida.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Emplea un encabezado azul brillante con texto blanco, contrastando fuertemente con el fondo blanco general de la página.</t>
+          <t>La paleta se centra en un azul brillante para la cabecera y el blanco para el contenido, generando una apariencia limpia y enfocada en los productos.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Considerar una paleta de colores más suave o usar el azul dominante de forma más estratégica, quizás para resaltar elementos importantes.</t>
+          <t>Explorar el uso de tonos complementarios sutiles para áreas interactivas, mejorando la jerarquía visual sin saturar el diseño existente.</t>
         </is>
       </c>
     </row>
@@ -537,251 +537,251 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Adopta un tono predominantemente funcional y formal, centrado en la transacción y la eficiencia para el usuario.</t>
+          <t>Adopta un tono semi-formal, equilibrando la profesionalidad de las transacciones con un lenguaje cercano para construir confianza con sus usuarios.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Mantiene un enfoque formal y directo, priorizando la información del producto y la simplicidad en la experiencia de compra.</t>
+          <t>Mantiene un tono predominantemente formal y transaccional, priorizando la claridad y eficiencia en la comunicación de detalles de productos y servicios.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Presenta un estilo juvenil y dinámico, utilizando un lenguaje cercano y amigable que fomenta una experiencia relajada y eficiente.</t>
+          <t>Utiliza un lenguaje muy informal y amigable, con emojis y expresiones coloquiales que reflejan la juventud y dinamismo de su público objetivo.</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Muestra un tono directo y funcional, centrado en la acción (aprender, armar, comparar) con un lenguaje técnico apropiado para su nicho.</t>
+          <t>Muestra un tono más formal y directo, enfocado en la funcionalidad y la información técnica, adecuado para un nicho de componentes tecnológicos.</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Introducir micro-interacciones lúdicas o un lenguaje más cercano en descripciones podría humanizar la experiencia sin perder formalidad.</t>
+          <t>Podría beneficiarse de introducir elementos de lenguaje ligeramente más conversacionales para fomentar mayor engagement con la comunidad de ensambladores.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Personajes / Iconos / Emblemas</t>
+          <t>Characters / Icons / Emblems</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Utiliza íconos claros y universales para la navegación, como carritos de compra y corazones, mejorando la usabilidad.</t>
+          <t>Su logo con la balanza y flecha simboliza comercio y eficiencia; los iconos son minimalistas y funcionales, facilitando la navegación sin distracciones.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Presenta íconos simples y directos, destacando la flecha debajo de su logo y los símbolos de categorías para una navegación intuitiva.</t>
+          <t>El logo con la flecha de la 'a' a la 'z' subraya su vasta oferta; los iconos son universales y muy reconocibles, promoviendo una interacción intuitiva.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Emplea un logotipo memorable y íconos modernos que refuerzan su identidad de marca, facilitando la identificación de secciones clave.</t>
+          <t>Usa un logo sencillo con un globo de diálogo y un tenedor, junto a iconos claros que representan categorías de comida y estados de pedidos.</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Integra un logo distintivo de ratón/procesador, íconos funcionales (búsqueda, usuario) y las imágenes de producto como elementos centrales.</t>
+          <t>El logo es una combinación de un ratón de PC con un embudo/circuito, y los iconos (lupa, persona) son estándar y claros, mejorando la usabilidad.</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Explorar animaciones sutiles para el logo o los íconos, o usar gráficos más expresivos para categorías, mejoraría el atractivo visual.</t>
+          <t>Desarrollar un conjunto de iconos personalizados y únicos que reflejen aún más la temática de construcción de PCs, añadiendo personalidad de marca.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Accesibilidad</t>
+          <t>Accessibility</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Se esfuerza por una interfaz accesible, con contrastes adecuados y elementos bien definidos para diversos usuarios.</t>
+          <t>Ofrece opciones como descripciones de imágenes y compatibilidad con lectores de pantalla, buscando ser inclusivo para usuarios con diversas capacidades.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Diseña pensando en la accesibilidad web, ofreciendo opciones para lectores de pantalla y navegación por teclado, promoviendo la inclusión.</t>
+          <t>Invierte en características de accesibilidad robustas, incluyendo navegación por teclado y soporte para texto de alto contraste, garantizando una experiencia para todos.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Asegura una navegación sencilla y una presentación clara, permitiendo que usuarios con diferentes capacidades interactúen eficazmente.</t>
+          <t>Se enfoca en una interfaz sencilla con grandes botones, facilitando el uso para usuarios con posibles dificultades motoras o visuales leves, priorizando la rapidez.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Ofrece un contraste visual fuerte entre el azul del encabezado y el blanco del contenido, facilitando la lectura general de la información.</t>
+          <t>La legibilidad del texto y el contraste de colores son adecuados, lo que sugiere una buena base para la accesibilidad general de la plataforma.</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Implementar mejoras en la navegación por teclado y asegurar descripciones alt para imágenes potenciaría significativamente la accesibilidad.</t>
+          <t>Implementar alternativas de texto para todas las imágenes y asegurar una navegación totalmente controlable por teclado para usuarios con discapacidades.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Navegación (botones importantes)</t>
+          <t>Navigation (important buttons)</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Botones claros para 'Comprar', 'Agregar al carrito' y filtros, facilitando la interacción rápida y eficiente del usuario.</t>
+          <t>Botones de "Comprar" y "Agregar al carrito" son prominentes, junto a una barra de búsqueda eficiente, guiando al usuario rápidamente hacia la compra.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Destaca botones como 'Añadir a la cesta', 'Comprar ahora' y categorías visibles, simplificando el proceso de compra.</t>
+          <t>Destaca por su navegación intuitiva con un mega-menú y botones de acción claros, permitiendo a los usuarios encontrar productos con facilidad.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Botones prominentes para 'Ver menú', 'Pedir ahora' y filtros de comida, guiando al usuario rápidamente a su elección.</t>
+          <t>Sus botones de "Pedir" y "Reordenar" son muy visibles, con categorías de restaurantes claras, facilitando la elección y confirmación rápida de pedidos.</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Presenta enlaces de navegación claros en el encabezado ('Arma tu PC', 'Comparar') y elementos de producto clickeables para exploración detallada.</t>
+          <t>Los botones "Información", "Arma tu PC", "Comparar" son claros en la cabecera, junto a un campo de búsqueda prominente para encontrar productos.</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Dar mayor prominencia visual a los botones de acción clave y asegurar su consistencia en todo el recorrido del usuario.</t>
+          <t>Mejorar la visibilidad de los botones de filtros y opciones de ordenamiento dentro de la sección de productos para una mejor exploración.</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Organización</t>
+          <t>Organization</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Estructura de categorías y subcategorías bien definida, junto con barras de búsqueda robustas para encontrar productos fácilmente.</t>
+          <t>La organización de productos por categorías, tiendas oficiales y secciones de ofertas es clara, permitiendo una búsqueda eficiente para los usuarios.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Organización jerárquica clara con amplias categorías, filtros detallados y resultados de búsqueda relevantes para una experiencia eficiente.</t>
+          <t>Utiliza una categorización detallada y filtros avanzados, organizando eficazmente millones de productos para una experiencia de compra personalizada y sencilla.</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Presenta restaurantes y opciones de comida por categorías, ubicación y ofertas, permitiendo una búsqueda rápida y efectiva.</t>
+          <t>La organización por tipo de cocina, promociones y distancia es eficiente, permitiendo a los usuarios descubrir y seleccionar restaurantes rápidamente.</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Organiza los productos en una cuadrícula clara bajo secciones como 'Componentes populares', apoyándose en una barra de búsqueda superior para encontrar elementos.</t>
+          <t>Presenta los "Componentes populares" de manera atractiva en cuadrícula, con títulos de productos claros, mostrando una organización lógica inicial.</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Añadir opciones de filtrado avanzadas por especificaciones y comparativas personalizadas mejoraría significativamente la experiencia del usuario.</t>
+          <t>Incluir más opciones de filtrado y ordenamiento detallado (por socket, generación, marca) para los componentes populares mejoraría la experiencia.</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Características Extra</t>
+          <t>Extra features</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Ofrece Mercado Crédito, envíos rápidos con Mercado Envíos y una plataforma de publicidad para vendedores.</t>
+          <t>Ofrece Mercado Puntos, envíos Flex, y un sistema de preguntas y respuestas, añadiendo valor a la experiencia de compra y fidelización del cliente.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Destaca suscripciones Prime con beneficios exclusivos, servicios en la nube (AWS) y una vasta oferta de productos digitales.</t>
+          <t>Presenta Amazon Prime, reseñas detalladas, listas de deseos y recomendaciones personalizadas, enriqueciendo significativamente la interacción del usuario.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Incluye seguimiento de pedidos en tiempo real, opciones de pago diversas y la posibilidad de programar entregas.</t>
+          <t>Dispone de seguimiento de pedidos en tiempo real, promociones exclusivas y la opción de calificar restaurantes, mejorando la conveniencia del servicio.</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Sus características destacadas son las herramientas 'Arma tu PC' y 'Comparar', esenciales para usuarios interesados en construir o evaluar equipos.</t>
+          <t>Ofrece "Arma tu PC" y "Comparar" como características distintivas, lo cual es muy útil para su audiencia especializada en hardware de computadoras.</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Integrar más profundamente las funciones de 'Arma tu PC' y 'Comparar' directamente en las fichas de producto facilitaría su uso.</t>
+          <t>Considerar la implementación de un foro comunitario o un blog con guías de ensamblaje para fomentar la interacción y educar a los usuarios.</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Tutoriales o Instrucciones</t>
+          <t>Tutorials or Instructions</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Proporciona centros de ayuda detallados y tutoriales para compradores y vendedores, cubriendo diversas operaciones.</t>
+          <t>Proporciona secciones de ayuda y guías para vendedores y compradores, facilitando el uso de la plataforma y resolviendo dudas comunes.</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Dispone de una extensa sección de ayuda, guías para el comprador y vendedor, y soporte al cliente para cualquier consulta.</t>
+          <t>Cuenta con amplias páginas de ayuda, tutoriales en video y descripciones detalladas de productos, asistiendo a los usuarios en cada etapa de su compra.</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Ofrece guías claras sobre cómo realizar pedidos, usar promociones y resolver problemas comunes de manera eficiente.</t>
+          <t>Sus instrucciones son simples y directas para realizar pedidos, con una sección de preguntas frecuentes que resuelve dudas básicas de manera eficiente.</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Posee un enlace 'Información' que probablemente dirige a tutoriales o guías de uso, esencial para el público técnico al que apunta.</t>
+          <t>La sección "Arma tu PC" sugiere que hay guías implícitas, pero una sección explícita de "Información" o "Ayuda" sería beneficiosa y más visible.</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Desarrollar tutoriales interactivos para guiar a los usuarios en el proceso de 'Arma tu PC' mejoraría la experiencia del novato.</t>
+          <t>Desarrollar una base de conocimientos completa con tutoriales detallados sobre la compatibilidad de componentes y guías de ensamblaje paso a paso.</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Impresión General del Sitio</t>
+          <t>Overall User Experience</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Proporciona una plataforma robusta y confiable para comercio electrónico, con un enfoque en la eficiencia transaccional y amplia variedad.</t>
+          <t>Ofrece una experiencia completa y funcional, con facilidad de compra y venta, aunque a veces la saturación de ofertas puede ser abrumadora.</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Se percibe como un gigante del e-commerce, ofreciendo conveniencia, una selección inmensa y servicios integrados.</t>
+          <t>Proporciona una UX pulida y eficiente, priorizando la comodidad y personalización, lo que permite a los usuarios encontrar y comprar con facilidad.</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Transmite una sensación de rapidez y conveniencia para la entrega de comida y productos, con una interfaz muy directa.</t>
+          <t>Se enfoca en una experiencia rápida y sin fricciones para pedir comida, con una interfaz intuitiva que minimiza los pasos necesarios para completar la orden.</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Ofrece una impresión de sitio especializado y funcional para hardware de PC, con una interfaz limpia y centrada en componentes.</t>
+          <t>La interfaz es limpia y enfocada, facilitando la visualización de componentes y la navegación básica para usuarios interesados en ensamblar PCs.</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Refinar los elementos visuales y expandir las herramientas de personalización podría solidificar su posición como referente en el nicho.</t>
+          <t>Optimizar los tiempos de carga de las páginas de productos y mejorar la retroalimentación visual en las interacciones para una experiencia más fluida.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
ARREGLE EL CREADOR DE IMGGG 💢
</commit_message>
<xml_diff>
--- a/IA/tablas_generadas/tablita.xlsx
+++ b/IA/tablas_generadas/tablita.xlsx
@@ -441,27 +441,27 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>mercado_libre</t>
+          <t>Mercado Libre</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>amazon</t>
+          <t>Amazon</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>pedidoya</t>
+          <t>PedidoYa</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>website_from_image</t>
+          <t>Website from Image</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>conclusion</t>
+          <t>Conclusion</t>
         </is>
       </c>
     </row>
@@ -473,27 +473,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Utiliza una tipografía Sans-serif clara y legible, como Arial o Open Sans, que asegura una buena experiencia de lectura en todos sus dispositivos.</t>
+          <t>Utiliza una tipografía sans-serif personalizada, con líneas suavizadas y redondeadas, para una legibilidad óptima y moderna en su plataforma. [8, 40]</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Emplea una tipografía distintiva (Amazon Ember) para mantener consistencia visual, facilitando la identificación de la marca y la lectura de descripciones de productos.</t>
+          <t>Emplea principalmente Amazon Ember, una sans-serif personalizada, que asegura una lectura clara y profesional en todos sus diversos dispositivos y plataformas. [5, 9, 14]</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Su tipografía es moderna y amigable, a menudo usando una fuente redondeada y sencilla para transmitir accesibilidad y rapidez en el servicio de entrega.</t>
+          <t>Muestra una tipografía sans-serif moderna y limpia en su interfaz, priorizando la claridad y facilidad de lectura para una experiencia de usuario eficiente. [33]</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>La tipografía es limpia y moderna, principalmente sans-serif, ofreciendo buena legibilidad para nombres de productos y encabezados importantes en la página.</t>
+          <t>Utiliza una tipografía sans-serif limpia y estándar, asegurando excelente legibilidad para títulos, descripciones y elementos de navegación de la página.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Considerar incorporar variaciones de peso o tamaño para destacar mejor elementos clave sin comprometer la consistencia global del sitio.</t>
+          <t>Explorar variaciones de fuentes que refuercen la identidad de la marca, manteniendo la claridad y adaptándose mejor a la estética tecnológica.</t>
         </is>
       </c>
     </row>
@@ -505,27 +505,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Domina el amarillo vibrante junto con el azul oscuro, creando un contraste energético que llama la atención y resalta ofertas especiales.</t>
+          <t>Su paleta distintiva combina amarillo brillante, azul profundo y blanco, simbolizando energía, confianza y una plataforma abierta para todos. [2, 3, 8, 19]</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Predominan el blanco, negro y un toque de naranja/azul, generando un esquema de colores profesional que facilita la concentración en los productos mostrados.</t>
+          <t>Predominan el naranja energético, el negro y el blanco; estos colores clave crean una identidad de marca reconocible y funcional en su interfaz. [1, 4, 6, 15]</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Se caracteriza por el rojo brillante y el blanco, transmitiendo energía y urgencia, lo cual es muy apropiado para su modelo de negocio de entrega rápida.</t>
+          <t>Ha evolucionado su paleta cromática con un enfoque moderno, usando colores vibrantes y frescos que reflejan su estrategia expansiva y espontánea. [11, 33]</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>La paleta se centra en un azul brillante para la cabecera y el blanco para el contenido, generando una apariencia limpia y enfocada en los productos.</t>
+          <t>La paleta principal es azul vibrante para el encabezado, blanco de fondo y negro para el texto, ofreciendo un contraste nítido y funcional.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Explorar el uso de tonos complementarios sutiles para áreas interactivas, mejorando la jerarquía visual sin saturar el diseño existente.</t>
+          <t>Introducir sutilmente colores secundarios para destacar llamadas a la acción o elementos interactivos podría mejorar la jerarquía visual del diseño.</t>
         </is>
       </c>
     </row>
@@ -537,27 +537,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Adopta un tono semi-formal, equilibrando la profesionalidad de las transacciones con un lenguaje cercano para construir confianza con sus usuarios.</t>
+          <t>Mantiene un equilibrio, con un diseño que transmite profesionalismo en transacciones y una accesibilidad amigable que fomenta la comunidad. [2, 8, 32]</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Mantiene un tono predominantemente formal y transaccional, priorizando la claridad y eficiencia en la comunicación de detalles de productos y servicios.</t>
+          <t>Su diseño es profesional y metódico, centrado en la eficiencia de la compra, aunque mantiene un tono accesible para el cliente. [5, 18, 31]</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Utiliza un lenguaje muy informal y amigable, con emojis y expresiones coloquiales que reflejan la juventud y dinamismo de su público objetivo.</t>
+          <t>Ha adoptado una estrategia más espontánea y abierta, inclinándose hacia un estilo informal que promueve cercanía y facilidad de uso. [33]</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Muestra un tono más formal y directo, enfocado en la funcionalidad y la información técnica, adecuado para un nicho de componentes tecnológicos.</t>
+          <t>El diseño es profesional y directo, centrado en la funcionalidad de comparación y armado de componentes de PC, transmitiendo seriedad.</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Podría beneficiarse de introducir elementos de lenguaje ligeramente más conversacionales para fomentar mayor engagement con la comunidad de ensambladores.</t>
+          <t>Adoptar un tono más amigable en descripciones o mensajes podría conectar mejor con usuarios menos técnicos, manteniendo profesionalismo.</t>
         </is>
       </c>
     </row>
@@ -569,27 +569,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Su logo con la balanza y flecha simboliza comercio y eficiencia; los iconos son minimalistas y funcionales, facilitando la navegación sin distracciones.</t>
+          <t>Presenta el icónico logotipo de dos manos estrechándose, que simboliza confianza, alianza y una sólida conexión dentro de su comunidad. [2, 8]</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>El logo con la flecha de la 'a' a la 'z' subraya su vasta oferta; los iconos son universales y muy reconocibles, promoviendo una interacción intuitiva.</t>
+          <t>Destaca por la flecha de la sonrisa que va de la 'A' a la 'Z' en su logo, sugiriendo variedad y la satisfacción completa del cliente. [5]</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Usa un logo sencillo con un globo de diálogo y un tenedor, junto a iconos claros que representan categorías de comida y estados de pedidos.</t>
+          <t>Utiliza un logotipo moderno que incluye elementos visuales distintivos, reforzando su identidad como una plataforma ágil de delivery. [45]</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>El logo es una combinación de un ratón de PC con un embudo/circuito, y los iconos (lupa, persona) son estándar y claros, mejorando la usabilidad.</t>
+          <t>Un logo de ratón estilizado con 'Rity', e iconos de búsqueda y perfil genéricos, son claros y funcionales.</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Desarrollar un conjunto de iconos personalizados y únicos que reflejen aún más la temática de construcción de PCs, añadiendo personalidad de marca.</t>
+          <t>El diseño de iconos más únicos o un emblema secundario podría reforzar la singularidad de la marca en el nicho tecnológico.</t>
         </is>
       </c>
     </row>
@@ -601,27 +601,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Ofrece opciones como descripciones de imágenes y compatibilidad con lectores de pantalla, buscando ser inclusivo para usuarios con diversas capacidades.</t>
+          <t>Integra funcionalidades para asegurar la usabilidad general, aunque detalles específicos de accesibilidad no fueron encontrados en la búsqueda. [2]</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Invierte en características de accesibilidad robustas, incluyendo navegación por teclado y soporte para texto de alto contraste, garantizando una experiencia para todos.</t>
+          <t>Ofrece extensas funciones como VoiceView, textos ajustables y descripciones de audio, garantizando que su plataforma sea inclusiva para todos los usuarios. [7, 12, 25, 31]</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Se enfoca en una interfaz sencilla con grandes botones, facilitando el uso para usuarios con posibles dificultades motoras o visuales leves, priorizando la rapidez.</t>
+          <t>Su rebranding abordó problemas previos de accesibilidad y contraste en la paleta de colores, buscando una mayor legibilidad para los usuarios. [33]</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>La legibilidad del texto y el contraste de colores son adecuados, lo que sugiere una buena base para la accesibilidad general de la plataforma.</t>
+          <t>La combinación de colores y tamaños de fuente ofrece buena legibilidad. No se aprecian características avanzadas de accesibilidad en la interfaz.</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Implementar alternativas de texto para todas las imágenes y asegurar una navegación totalmente controlable por teclado para usuarios con discapacidades.</t>
+          <t>Implementar opciones de contraste alto o herramientas de lectura de pantalla mejoraría la experiencia para usuarios con diversas necesidades visuales.</t>
         </is>
       </c>
     </row>
@@ -633,27 +633,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Botones de "Comprar" y "Agregar al carrito" son prominentes, junto a una barra de búsqueda eficiente, guiando al usuario rápidamente hacia la compra.</t>
+          <t>Cuenta con una interfaz de usuario intuitiva que guía a los usuarios, con botones clave para búsquedas y gestión de compras, facilitando el recorrido. [2]</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Destaca por su navegación intuitiva con un mega-menú y botones de acción claros, permitiendo a los usuarios encontrar productos con facilidad.</t>
+          <t>Tiene una navegación fluida con una barra de búsqueda central, botones de compra rápida y un menú claro para explorar amplias categorías de productos. [18, 21, 31]</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Sus botones de "Pedir" y "Reordenar" son muy visibles, con categorías de restaurantes claras, facilitando la elección y confirmación rápida de pedidos.</t>
+          <t>Ofrece una navegación sencilla, con botones destacados para pedidos, seguimiento y opciones de cuenta, optimizando la experiencia de entrega rápida.</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Los botones "Información", "Arma tu PC", "Comparar" son claros en la cabecera, junto a un campo de búsqueda prominente para encontrar productos.</t>
+          <t>La barra superior presenta enlaces vitales: 'Información', 'Arma tu PC', 'Comparar', y una barra de búsqueda prominente.</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Mejorar la visibilidad de los botones de filtros y opciones de ordenamiento dentro de la sección de productos para una mejor exploración.</t>
+          <t>Una disposición mejorada de los elementos clave, destacando 'Arma tu PC', podría optimizar el flujo de usuarios.</t>
         </is>
       </c>
     </row>
@@ -665,27 +665,27 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>La organización de productos por categorías, tiendas oficiales y secciones de ofertas es clara, permitiendo una búsqueda eficiente para los usuarios.</t>
+          <t>Opera con una estructura jerárquica y funcional, con divisiones claras en tecnología, operaciones y finanzas, optimizando su gestión regional. [27, 29, 43]</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Utiliza una categorización detallada y filtros avanzados, organizando eficazmente millones de productos para una experiencia de compra personalizada y sencilla.</t>
+          <t>Presenta una estructura organizacional funcional y jerárquica, con equipos especializados en funciones y divisiones geográficas, permitiendo una gestión global eficiente. [23, 24, 35]</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>La organización por tipo de cocina, promociones y distancia es eficiente, permitiendo a los usuarios descubrir y seleccionar restaurantes rápidamente.</t>
+          <t>Como parte de Delivery Hero, su organización interna se enfoca en la eficiencia operativa para gestionar entregas en múltiples mercados. [47]</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Presenta los "Componentes populares" de manera atractiva en cuadrícula, con títulos de productos claros, mostrando una organización lógica inicial.</t>
+          <t>La página está organizada con un encabezado fijo, título principal y componentes populares en un diseño de cuadrícula estructurada.</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Incluir más opciones de filtrado y ordenamiento detallado (por socket, generación, marca) para los componentes populares mejoraría la experiencia.</t>
+          <t>Añadir filtros o categorías claras para los componentes populares facilitaría la exploración y la búsqueda de productos específicos.</t>
         </is>
       </c>
     </row>
@@ -697,27 +697,27 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Ofrece Mercado Puntos, envíos Flex, y un sistema de preguntas y respuestas, añadiendo valor a la experiencia de compra y fidelización del cliente.</t>
+          <t>Ofrece un ecosistema integral de servicios como Mercado Pago y Mercado Envíos, expandiendo sus capacidades más allá de las compras básicas. [2]</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Presenta Amazon Prime, reseñas detalladas, listas de deseos y recomendaciones personalizadas, enriqueciendo significativamente la interacción del usuario.</t>
+          <t>Destaca por sus recomendaciones personalizadas, pedidos con un clic, y características innovadoras como Amazon Go y el asistente virtual Alexa. [20, 21, 31]</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Dispone de seguimiento de pedidos en tiempo real, promociones exclusivas y la opción de calificar restaurantes, mejorando la conveniencia del servicio.</t>
+          <t>Permite el seguimiento de pedidos en tiempo real, opciones de pago variadas y personalización de pedidos, enriqueciendo la experiencia de delivery.</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Ofrece "Arma tu PC" y "Comparar" como características distintivas, lo cual es muy útil para su audiencia especializada en hardware de computadoras.</t>
+          <t>Las funciones de 'Arma tu PC' y 'Comparar' indican herramientas interactivas avanzadas para configurar y evaluar hardware.</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Considerar la implementación de un foro comunitario o un blog con guías de ensamblaje para fomentar la interacción y educar a los usuarios.</t>
+          <t>Destacar visiblemente las características únicas como 'Arma tu PC' con descripciones claras invitaría a más usuarios a explorarlas.</t>
         </is>
       </c>
     </row>
@@ -729,59 +729,59 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Proporciona secciones de ayuda y guías para vendedores y compradores, facilitando el uso de la plataforma y resolviendo dudas comunes.</t>
+          <t>La plataforma integra guías claras para vendedores sobre cómo usar sus herramientas, lo que facilita la creación y gestión de tiendas online. [44]</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Cuenta con amplias páginas de ayuda, tutoriales en video y descripciones detalladas de productos, asistiendo a los usuarios en cada etapa de su compra.</t>
+          <t>Proporciona una bienvenida opcional para nuevos usuarios y asistentes de voz que incluyen tutoriales en pantalla, facilitando la adaptación del usuario. [20, 28]</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Sus instrucciones son simples y directas para realizar pedidos, con una sección de preguntas frecuentes que resuelve dudas básicas de manera eficiente.</t>
+          <t>Incorpora instrucciones sencillas para realizar pedidos, personalizar entregas y utilizar las funcionalidades de la aplicación de manera intuitiva.</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>La sección "Arma tu PC" sugiere que hay guías implícitas, pero una sección explícita de "Información" o "Ayuda" sería beneficiosa y más visible.</t>
+          <t>El título 'Aprendé, Armá y Compará' sugiere una sección educativa, aunque no hay tutoriales explícitos visibles aquí.</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Desarrollar una base de conocimientos completa con tutoriales detallados sobre la compatibilidad de componentes y guías de ensamblaje paso a paso.</t>
+          <t>Ofrecer mini-guías o tooltips interactivos sobre cómo usar las funciones de armado y comparación podría enriquecer la experiencia.</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Overall User Experience</t>
+          <t>User Interface Cohesion</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Ofrece una experiencia completa y funcional, con facilidad de compra y venta, aunque a veces la saturación de ofertas puede ser abrumadora.</t>
+          <t>A pesar de una arquitectura inicial fragmentada, ha logrado una identidad unificada con elementos visuales consistentes en todo su ecosistema. [2, 44]</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Proporciona una UX pulida y eficiente, priorizando la comodidad y personalización, lo que permite a los usuarios encontrar y comprar con facilidad.</t>
+          <t>Posee una cohesión de interfaz excepcional, manteniendo un diseño limpio y consistente en el sitio web, aplicaciones y materiales de marketing globalmente. [5, 18, 31]</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Se enfoca en una experiencia rápida y sin fricciones para pedir comida, con una interfaz intuitiva que minimiza los pasos necesarios para completar la orden.</t>
+          <t>Su reciente proceso de rebranding buscó una identidad visual más holística, unificando la experiencia en todas sus plataformas digitales. [33]</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>La interfaz es limpia y enfocada, facilitando la visualización de componentes y la navegación básica para usuarios interesados en ensamblar PCs.</t>
+          <t>El diseño demuestra consistencia en tipografía, colores y disposición de elementos, generando una experiencia visual unificada y ordenada.</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Optimizar los tiempos de carga de las páginas de productos y mejorar la retroalimentación visual en las interacciones para una experiencia más fluida.</t>
+          <t>Reforzar la identidad visual con elementos gráficos recurrentes, quizás en los cuadros de producto, podría aumentar la sensación de marca.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
arrelgo de conclusiones para el usuario. falta ajustar la tabla
</commit_message>
<xml_diff>
--- a/IA/tablas_generadas/tablita.xlsx
+++ b/IA/tablas_generadas/tablita.xlsx
@@ -436,32 +436,32 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>criterion</t>
+          <t>criterion_or_website</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Mercado Libre</t>
+          <t>website_1_value</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Amazon</t>
+          <t>website_2_value</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>PedidoYa</t>
+          <t>website_3_value</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Website from Image</t>
+          <t>website_4_value</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Conclusion</t>
+          <t>conclusion</t>
         </is>
       </c>
     </row>
@@ -473,27 +473,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Utiliza una tipografía sans-serif personalizada, con líneas suavizadas y redondeadas, para una legibilidad óptima y moderna en su plataforma. [8, 40]</t>
+          <t>Utiliza fuentes sans-serif claras y legibles, como Segoe UI, con una jerarquía consistente para títulos y texto principal.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Emplea principalmente Amazon Ember, una sans-serif personalizada, que asegura una lectura clara y profesional en todos sus diversos dispositivos y plataformas. [5, 9, 14]</t>
+          <t>Emplea tipografías sans-serif modernas y limpias, priorizando la legibilidad en subtítulos y descripciones de fotos.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Muestra una tipografía sans-serif moderna y limpia en su interfaz, priorizando la claridad y facilidad de lectura para una experiencia de usuario eficiente. [33]</t>
+          <t>Fuentes sans-serif profesionales como Open Sans, garantizando alta legibilidad para contenido empresarial y perfiles detallados.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Utiliza una tipografía sans-serif limpia y estándar, asegurando excelente legibilidad para títulos, descripciones y elementos de navegación de la página.</t>
+          <t>Tipografía sans-serif estándar y sencilla, lo que asegura buena legibilidad para nombres de productos y títulos.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Explorar variaciones de fuentes que refuercen la identidad de la marca, manteniendo la claridad y adaptándose mejor a la estética tecnológica.</t>
+          <t>Podría explorar una tipografía más distintiva o una paleta de fuentes complementarias para añadir carácter y diferenciación visual.</t>
         </is>
       </c>
     </row>
@@ -505,27 +505,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Su paleta distintiva combina amarillo brillante, azul profundo y blanco, simbolizando energía, confianza y una plataforma abierta para todos. [2, 3, 8, 19]</t>
+          <t>Predominan azules y blancos, transmitiendo confianza y familiaridad, con un contraste elevado para la lectura.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Predominan el naranja energético, el negro y el blanco; estos colores clave crean una identidad de marca reconocible y funcional en su interfaz. [1, 4, 6, 15]</t>
+          <t>Logo con gradientes vibrantes, interfaz principalmente blanca y texto negro, destacando el contenido visual.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Ha evolucionado su paleta cromática con un enfoque moderno, usando colores vibrantes y frescos que reflejan su estrategia expansiva y espontánea. [11, 33]</t>
+          <t>Esquema de colores corporativos: azul, blanco y gris, que proyecta profesionalismo y un entorno de trabajo serio.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>La paleta principal es azul vibrante para el encabezado, blanco de fondo y negro para el texto, ofreciendo un contraste nítido y funcional.</t>
+          <t>Dominante cabecera azul brillante con texto blanco, cuerpo de la página blanco con texto negro, colores funcionales.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Introducir sutilmente colores secundarios para destacar llamadas a la acción o elementos interactivos podría mejorar la jerarquía visual del diseño.</t>
+          <t>La paleta de colores es básica; considerar introducir un color secundario o acentos para destacar elementos clave y mejorar la estética general.</t>
         </is>
       </c>
     </row>
@@ -537,27 +537,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Mantiene un equilibrio, con un diseño que transmite profesionalismo en transacciones y una accesibilidad amigable que fomenta la comunidad. [2, 8, 32]</t>
+          <t>Mezcla de tono, más informal para interacciones personales y algo formal para noticias y páginas oficiales.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Su diseño es profesional y metódico, centrado en la eficiencia de la compra, aunque mantiene un tono accesible para el cliente. [5, 18, 31]</t>
+          <t>Predominantemente informal y visual, centrado en la expresión creativa y estilos de vida personales.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Ha adoptado una estrategia más espontánea y abierta, inclinándose hacia un estilo informal que promueve cercanía y facilidad de uso. [33]</t>
+          <t>Estrictamente formal y profesional, diseñado para networking, búsqueda de empleo y desarrollo de negocios.</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>El diseño es profesional y directo, centrado en la funcionalidad de comparación y armado de componentes de PC, transmitiendo seriedad.</t>
+          <t>Tono formal y funcional, típico de sitios de comercio electrónico y utilidades, enfocado en información de productos.</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Adoptar un tono más amigable en descripciones o mensajes podría conectar mejor con usuarios menos técnicos, manteniendo profesionalismo.</t>
+          <t>El tono es adecuado para una tienda de componentes; sin embargo, un toque sutil de calidez podría mejorar la conexión con el usuario.</t>
         </is>
       </c>
     </row>
@@ -569,27 +569,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Presenta el icónico logotipo de dos manos estrechándose, que simboliza confianza, alianza y una sólida conexión dentro de su comunidad. [2, 8]</t>
+          <t>Íconos universales de redes sociales, botones de 'me gusta', perfiles de usuario y emoticonos reconocibles.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Destaca por la flecha de la sonrisa que va de la 'A' a la 'Z' en su logo, sugiriendo variedad y la satisfacción completa del cliente. [5]</t>
+          <t>Íconos minimalistas (corazón, burbuja de diálogo, avión de papel), con énfasis en las imágenes de perfil de usuario.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Utiliza un logotipo moderno que incluye elementos visuales distintivos, reforzando su identidad como una plataforma ágil de delivery. [45]</t>
+          <t>Íconos profesionales para conexiones, empleos y mensajes, junto con logotipos de empresas y fotos de perfil.</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Un logo de ratón estilizado con 'Rity', e iconos de búsqueda y perfil genéricos, son claros y funcionales.</t>
+          <t>Íconos simples y funcionales: búsqueda, perfil de usuario y un logo de ratón 'PMCity' claro y directo en la cabecera.</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>El diseño de iconos más únicos o un emblema secundario podría reforzar la singularidad de la marca en el nicho tecnológico.</t>
+          <t>Los íconos son funcionales pero sencillos; mejorar el diseño del logo y considerar íconos más modernos y coherentes visualmente.</t>
         </is>
       </c>
     </row>
@@ -601,27 +601,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Integra funcionalidades para asegurar la usabilidad general, aunque detalles específicos de accesibilidad no fueron encontrados en la búsqueda. [2]</t>
+          <t>Generalmente buena accesibilidad con texto alternativo para imágenes y navegación por teclado bien implementada.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Ofrece extensas funciones como VoiceView, textos ajustables y descripciones de audio, garantizando que su plataforma sea inclusiva para todos los usuarios. [7, 12, 25, 31]</t>
+          <t>Accesibilidad básica, incluyendo texto alternativo para fotos y soporte para lectores de pantalla en ciertas funciones.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Su rebranding abordó problemas previos de accesibilidad y contraste en la paleta de colores, buscando una mayor legibilidad para los usuarios. [33]</t>
+          <t>Buenas prácticas de accesibilidad, estructura semántica clara y navegación por teclado robusta para profesionales.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>La combinación de colores y tamaños de fuente ofrece buena legibilidad. No se aprecian características avanzadas de accesibilidad en la interfaz.</t>
+          <t>Aparentemente buen contraste de texto y navegación clara. No se observan barreras obvias en la interfaz visible.</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Implementar opciones de contraste alto o herramientas de lectura de pantalla mejoraría la experiencia para usuarios con diversas necesidades visuales.</t>
+          <t>Asegurar que todos los elementos interactivos sean navegables por teclado y que las imágenes de productos incluyan descripciones de texto alternativo.</t>
         </is>
       </c>
     </row>
@@ -633,27 +633,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Cuenta con una interfaz de usuario intuitiva que guía a los usuarios, con botones clave para búsquedas y gestión de compras, facilitando el recorrido. [2]</t>
+          <t>Barra superior con secciones (Inicio, Watch, Marketplace), barra lateral extensa y barra de búsqueda prominentemente.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Tiene una navegación fluida con una barra de búsqueda central, botones de compra rápida y un menú claro para explorar amplias categorías de productos. [18, 21, 31]</t>
+          <t>Barra de navegación inferior intuitiva (Inicio, Buscar, Reels, Tienda, Perfil) y botones superiores para mensajes.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Ofrece una navegación sencilla, con botones destacados para pedidos, seguimiento y opciones de cuenta, optimizando la experiencia de entrega rápida.</t>
+          <t>Navegación superior global (Inicio, Mi red, Empleos) y un menú de perfil claro, estructurado para uso profesional.</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>La barra superior presenta enlaces vitales: 'Información', 'Arma tu PC', 'Comparar', y una barra de búsqueda prominente.</t>
+          <t>Cabecera con enlaces 'Información', 'Arma tu PC', 'Comparar' y una barra de búsqueda visible, navegación directa.</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Una disposición mejorada de los elementos clave, destacando 'Arma tu PC', podría optimizar el flujo de usuarios.</t>
+          <t>La navegación principal es clara; se podría añadir un 'carrito' de compras o un historial de búsquedas para mejorar la experiencia del usuario.</t>
         </is>
       </c>
     </row>
@@ -665,27 +665,27 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Opera con una estructura jerárquica y funcional, con divisiones claras en tecnología, operaciones y finanzas, optimizando su gestión regional. [27, 29, 43]</t>
+          <t>Organización basada en un 'feed' de noticias, secciones para grupos, páginas y perfiles personales.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Presenta una estructura organizacional funcional y jerárquica, con equipos especializados en funciones y divisiones geográficas, permitiendo una gestión global eficiente. [23, 24, 35]</t>
+          <t>Perfiles en cuadrícula, 'feed' y 'stories'; organización visual que enfatiza la disposición y el descubrimiento de contenido.</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Como parte de Delivery Hero, su organización interna se enfoca en la eficiencia operativa para gestionar entregas en múltiples mercados. [47]</t>
+          <t>Centrado en el perfil, 'feed' de noticias, listados de empleo y páginas de empresa, con secciones estructuradas para datos profesionales.</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>La página está organizada con un encabezado fijo, título principal y componentes populares en un diseño de cuadrícula estructurada.</t>
+          <t>Cabecera, título principal y sección de 'Componentes populares' en un diseño de cuadrícula claro y simple para productos.</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Añadir filtros o categorías claras para los componentes populares facilitaría la exploración y la búsqueda de productos específicos.</t>
+          <t>La organización es lógica para productos; considerar filtros de búsqueda avanzada y categorización de componentes para facilitar la exploración.</t>
         </is>
       </c>
     </row>
@@ -697,27 +697,27 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Ofrece un ecosistema integral de servicios como Mercado Pago y Mercado Envíos, expandiendo sus capacidades más allá de las compras básicas. [2]</t>
+          <t>Messenger, Marketplace, Grupos, Eventos, Juegos y transmisiones en vivo, ofreciendo un amplio conjunto de funciones.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Destaca por sus recomendaciones personalizadas, pedidos con un clic, y características innovadoras como Amazon Go y el asistente virtual Alexa. [20, 21, 31]</t>
+          <t>Reels, Stories, IGTV, Tienda y Live, un conjunto robusto de funciones para compartir y consumir contenido multimedia.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Permite el seguimiento de pedidos en tiempo real, opciones de pago variadas y personalización de pedidos, enriqueciendo la experiencia de delivery.</t>
+          <t>Búsqueda de empleo, LinkedIn Learning, artículos profesionales y grupos temáticos, herramientas profesionales completas.</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Las funciones de 'Arma tu PC' y 'Comparar' indican herramientas interactivas avanzadas para configurar y evaluar hardware.</t>
+          <t>'Arma tu PC' y 'Comparar', funciones muy relevantes para su propósito, que añaden valor directo al usuario.</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Destacar visiblemente las características únicas como 'Arma tu PC' con descripciones claras invitaría a más usuarios a explorarlas.</t>
+          <t>Las funciones de 'Arma tu PC' y 'Comparar' son excelentes; se podría integrar un sistema de reseñas de usuarios o foros para productos.</t>
         </is>
       </c>
     </row>
@@ -729,59 +729,59 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>La plataforma integra guías claras para vendedores sobre cómo usar sus herramientas, lo que facilita la creación y gestión de tiendas online. [44]</t>
+          <t>Centro de ayuda extenso con guías detalladas para funciones, consejos de seguridad y normas comunitarias.</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Proporciona una bienvenida opcional para nuevos usuarios y asistentes de voz que incluyen tutoriales en pantalla, facilitando la adaptación del usuario. [20, 28]</t>
+          <t>Centro de ayuda, guías para usar funciones como Reels o Stories, y configuración de privacidad.</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Incorpora instrucciones sencillas para realizar pedidos, personalizar entregas y utilizar las funcionalidades de la aplicación de manera intuitiva.</t>
+          <t>LinkedIn Learning (premium), extenso centro de ayuda y artículos de consejos profesionales y guías de uso.</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>El título 'Aprendé, Armá y Compará' sugiere una sección educativa, aunque no hay tutoriales explícitos visibles aquí.</t>
+          <t>La sección 'Aprende' sugiere contenido educativo, y la función 'Arma tu PC' actúa como un tutorial guiado de construcción.</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Ofrecer mini-guías o tooltips interactivos sobre cómo usar las funciones de armado y comparación podría enriquecer la experiencia.</t>
+          <t>Sería beneficioso incluir tutoriales de montaje o guías detalladas para principiantes, accesibles directamente desde las secciones 'Aprende' o 'Información'.</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>User Interface Cohesion</t>
+          <t>Overall User Experience</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>A pesar de una arquitectura inicial fragmentada, ha logrado una identidad unificada con elementos visuales consistentes en todo su ecosistema. [2, 44]</t>
+          <t>Experiencia integral, pero puede ser abrumadora por la cantidad de funciones, aunque intuitiva en lo básico.</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Posee una cohesión de interfaz excepcional, manteniendo un diseño limpio y consistente en el sitio web, aplicaciones y materiales de marketing globalmente. [5, 18, 31]</t>
+          <t>Muy atractiva y visual, intuitiva para compartir medios, pero puede generar sobrecarga de contenido visual.</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Su reciente proceso de rebranding buscó una identidad visual más holística, unificando la experiencia en todas sus plataformas digitales. [33]</t>
+          <t>Enfocada y eficiente para uso profesional, con rutas claras para networking y búsqueda de empleo, a veces algo formal.</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>El diseño demuestra consistencia en tipografía, colores y disposición de elementos, generando una experiencia visual unificada y ordenada.</t>
+          <t>Directa y funcional para encontrar componentes de PC, con un diseño limpio y sencillo para navegar fácilmente por los productos.</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Reforzar la identidad visual con elementos gráficos recurrentes, quizás en los cuadros de producto, podría aumentar la sensación de marca.</t>
+          <t>Para mejorar la experiencia general, optimizar los tiempos de carga de imágenes y añadir animaciones sutiles a las interacciones clave.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
quedó re piola la img ahora 💯
</commit_message>
<xml_diff>
--- a/IA/tablas_generadas/tablita.xlsx
+++ b/IA/tablas_generadas/tablita.xlsx
@@ -473,27 +473,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Utiliza fuentes sans-serif claras y legibles, como Segoe UI, con una jerarquía consistente para títulos y texto principal.</t>
+          <t>Utiliza Facebook Sans, una tipografía Sans-serif clara y legible, priorizando la coherencia en sus interfaces. [3]</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Emplea tipografías sans-serif modernas y limpias, priorizando la legibilidad en subtítulos y descripciones de fotos.</t>
+          <t>Presenta una combinación de fuentes limpias para texto estándar, con opciones creativas para historias y gráficos. [5, 8]</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Fuentes sans-serif profesionales como Open Sans, garantizando alta legibilidad para contenido empresarial y perfiles detallados.</t>
+          <t>Muestra tipografías audaces y dinámicas, a menudo con efectos visuales, reflejando su naturaleza juvenil y enérgica. [2, 4, 14, 17]</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Tipografía sans-serif estándar y sencilla, lo que asegura buena legibilidad para nombres de productos y títulos.</t>
+          <t>La tipografía es funcional pero carece de un estilo distintivo, usando fuentes estándar sin mucha personalidad ni jerarquía visual clara. [11, 20]</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Podría explorar una tipografía más distintiva o una paleta de fuentes complementarias para añadir carácter y diferenciación visual.</t>
+          <t>Considerar implementar una tipografía más moderna y única para diferenciar la marca visualmente y mejorar la jerarquía.</t>
         </is>
       </c>
     </row>
@@ -505,27 +505,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Predominan azules y blancos, transmitiendo confianza y familiaridad, con un contraste elevado para la lectura.</t>
+          <t>Dominan los tonos azules clásicos y blanco, proyectando profesionalismo, confianza y una sensación de familiaridad. [15]</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Logo con gradientes vibrantes, interfaz principalmente blanca y texto negro, destacando el contenido visual.</t>
+          <t>Se caracteriza por degradados vibrantes y colores cálidos, evocando creatividad, alegría y una estética moderna y atractiva. [8]</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Esquema de colores corporativos: azul, blanco y gris, que proyecta profesionalismo y un entorno de trabajo serio.</t>
+          <t>Emplea una paleta de colores oscuros y neón, generando una atmósfera moderna, juvenil y energéticamente estimulante. [1]</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Dominante cabecera azul brillante con texto blanco, cuerpo de la página blanco con texto negro, colores funcionales.</t>
+          <t>La paleta de colores es básica y monocromática, lo que resulta en una apariencia algo genérica, plana y sin vida. [7, 11]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>La paleta de colores es básica; considerar introducir un color secundario o acentos para destacar elementos clave y mejorar la estética general.</t>
+          <t>Introducir una paleta de colores más rica y atractiva que refuerce la identidad de la plataforma y el contraste.</t>
         </is>
       </c>
     </row>
@@ -537,27 +537,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Mezcla de tono, más informal para interacciones personales y algo formal para noticias y páginas oficiales.</t>
+          <t>Adopta un tono predominantemente semi-formal, adecuado para conexiones personales, profesionales y comunicados oficiales. [13, 19]</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Predominantemente informal y visual, centrado en la expresión creativa y estilos de vida personales.</t>
+          <t>Mantiene un estilo informal y visualmente atractivo, fomentando la expresión personal y la interacción casual entre usuarios. [5, 8]</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Estrictamente formal y profesional, diseñado para networking, búsqueda de empleo y desarrollo de negocios.</t>
+          <t>Opera en un registro marcadamente informal y lúdico, celebrando la espontaneidad y el entretenimiento sin filtros. [2, 14]</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Tono formal y funcional, típico de sitios de comercio electrónico y utilidades, enfocado en información de productos.</t>
+          <t>El lenguaje y el diseño son neutrales, cayendo en un rango formal que puede percibirse como poco cercano para el usuario. [6, 7]</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>El tono es adecuado para una tienda de componentes; sin embargo, un toque sutil de calidez podría mejorar la conexión con el usuario.</t>
+          <t>Evaluar un enfoque más informal en el lenguaje y diseño para fomentar mayor cercanía y participación activa de la audiencia.</t>
         </is>
       </c>
     </row>
@@ -569,27 +569,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Íconos universales de redes sociales, botones de 'me gusta', perfiles de usuario y emoticonos reconocibles.</t>
+          <t>Usa iconos planos y reconocibles universalmente, junto a un logo 'f' icónico y reacciones emotivas en el contenido. [12, 13, 15]</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Íconos minimalistas (corazón, burbuja de diálogo, avión de papel), con énfasis en las imágenes de perfil de usuario.</t>
+          <t>Destaca por sus iconos minimalistas, el logo de la cámara fotográfica retro y elementos visuales para historias y reels. [5, 8]</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Íconos profesionales para conexiones, empleos y mensajes, junto con logotipos de empresas y fotos de perfil.</t>
+          <t>Presenta iconos dinámicos y un emblema vibrante que resuenan con su audiencia joven y la cultura de videos cortos. [1]</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Íconos simples y funcionales: búsqueda, perfil de usuario y un logo de ratón 'PMCity' claro y directo en la cabecera.</t>
+          <t>Los iconos son genéricos y poco memorables, careciendo de un estilo unificado o elementos emblemáticos propios. [7]</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Los íconos son funcionales pero sencillos; mejorar el diseño del logo y considerar íconos más modernos y coherentes visualmente.</t>
+          <t>Desarrollar un conjunto de iconos personalizados y un emblema único que reflejen mejor la personalidad del sitio.</t>
         </is>
       </c>
     </row>
@@ -601,27 +601,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Generalmente buena accesibilidad con texto alternativo para imágenes y navegación por teclado bien implementada.</t>
+          <t>Ofrece múltiples funciones de accesibilidad, incluyendo lectores de pantalla y opciones de contraste para usuarios. [12]</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Accesibilidad básica, incluyendo texto alternativo para fotos y soporte para lectores de pantalla en ciertas funciones.</t>
+          <t>Ha mejorado su accesibilidad con texto alternativo para imágenes y subtítulos, aunque tiene áreas de oportunidad. [5, 8, 18]</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Buenas prácticas de accesibilidad, estructura semántica clara y navegación por teclado robusta para profesionales.</t>
+          <t>Continúa mejorando características de accesibilidad como subtítulos automáticos y ajustes de texto para inclusión plena. [1]</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Aparentemente buen contraste de texto y navegación clara. No se observan barreras obvias en la interfaz visible.</t>
+          <t>La accesibilidad es básica, con limitaciones en opciones de contraste, texto alternativo y navegación por teclado, dificultando el acceso. [10, 11]</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Asegurar que todos los elementos interactivos sean navegables por teclado y que las imágenes de productos incluyan descripciones de texto alternativo.</t>
+          <t>Implementar un conjunto robusto de características de accesibilidad para garantizar un uso inclusivo para todos.</t>
         </is>
       </c>
     </row>
@@ -633,27 +633,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Barra superior con secciones (Inicio, Watch, Marketplace), barra lateral extensa y barra de búsqueda prominentemente.</t>
+          <t>Posee una barra de navegación superior clara con accesos directos intuitivos a inicio, amigos y notificaciones. [19]</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Barra de navegación inferior intuitiva (Inicio, Buscar, Reels, Tienda, Perfil) y botones superiores para mensajes.</t>
+          <t>Cuenta con una barra inferior prominente para inicio, búsqueda, reels, tienda y perfil, facilitando el acceso rápido. [5]</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Navegación superior global (Inicio, Mi red, Empleos) y un menú de perfil claro, estructurado para uso profesional.</t>
+          <t>Su navegación se centra en un feed vertical infinito, con botones clave de inicio, seguir, crear y perfil. [1]</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Cabecera con enlaces 'Información', 'Arma tu PC', 'Comparar' y una barra de búsqueda visible, navegación directa.</t>
+          <t>Los botones de navegación son estándar y su jerarquía no es siempre clara, lo que puede confundir al usuario. [6, 7, 10]</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>La navegación principal es clara; se podría añadir un 'carrito' de compras o un historial de búsquedas para mejorar la experiencia del usuario.</t>
+          <t>Rediseñar la navegación para que los botones importantes sean más intuitivos, visibles y con una jerarquía clara.</t>
         </is>
       </c>
     </row>
@@ -665,27 +665,27 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Organización basada en un 'feed' de noticias, secciones para grupos, páginas y perfiles personales.</t>
+          <t>Estructura el contenido en un feed central y barras laterales para amigos/grupos, manteniendo la información organizada. [19]</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Perfiles en cuadrícula, 'feed' y 'stories'; organización visual que enfatiza la disposición y el descubrimiento de contenido.</t>
+          <t>Organiza el contenido de forma visual, priorizando cuadrículas de fotos, historias efímeras y reels de videos cortos. [5]</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Centrado en el perfil, 'feed' de noticias, listados de empleo y páginas de empresa, con secciones estructuradas para datos profesionales.</t>
+          <t>Su organización se basa en un algoritmo que personaliza el feed, presentando videos relevantes sin estructura rígida. [1]</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Cabecera, título principal y sección de 'Componentes populares' en un diseño de cuadrícula claro y simple para productos.</t>
+          <t>La organización del contenido es lineal y predecible, careciendo de dinamismo o personalización para el usuario. [7, 11]</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>La organización es lógica para productos; considerar filtros de búsqueda avanzada y categorización de componentes para facilitar la exploración.</t>
+          <t>Explorar nuevas formas de organizar el contenido, quizás con personalización, para mejorar la experiencia del usuario.</t>
         </is>
       </c>
     </row>
@@ -697,27 +697,27 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Messenger, Marketplace, Grupos, Eventos, Juegos y transmisiones en vivo, ofreciendo un amplio conjunto de funciones.</t>
+          <t>Ofrece Marketplace, Grupos, Eventos y Páginas, enriqueciendo la interacción y expandiendo las funcionalidades. [19]</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Reels, Stories, IGTV, Tienda y Live, un conjunto robusto de funciones para compartir y consumir contenido multimedia.</t>
+          <t>Incluye Stories, Reels, IGTV y la posibilidad de comprar directamente desde la aplicación, diversificando la experiencia. [5]</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Búsqueda de empleo, LinkedIn Learning, artículos profesionales y grupos temáticos, herramientas profesionales completas.</t>
+          <t>Destaca por sus herramientas de edición de video, filtros creativos, efectos AR y duetos interactivos para usuarios. [1]</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>'Arma tu PC' y 'Comparar', funciones muy relevantes para su propósito, que añaden valor directo al usuario.</t>
+          <t>Las características adicionales son mínimas o inexistentes, limitando la profundidad y la variedad de interacción del usuario.</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Las funciones de 'Arma tu PC' y 'Comparar' son excelentes; se podría integrar un sistema de reseñas de usuarios o foros para productos.</t>
+          <t>Desarrollar e integrar características adicionales innovadoras que aporten valor y diferenciación a la plataforma.</t>
         </is>
       </c>
     </row>
@@ -729,59 +729,59 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Centro de ayuda extenso con guías detalladas para funciones, consejos de seguridad y normas comunitarias.</t>
+          <t>Proporciona secciones de ayuda extensas y guías paso a paso para todas sus funcionalidades y herramientas complejas. [19]</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Centro de ayuda, guías para usar funciones como Reels o Stories, y configuración de privacidad.</t>
+          <t>Ofrece tutoriales integrados para nuevas funciones y un centro de ayuda robusto con preguntas frecuentes claras. [5, 8]</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>LinkedIn Learning (premium), extenso centro de ayuda y artículos de consejos profesionales y guías de uso.</t>
+          <t>Brinda guías visuales y consejos en la aplicación, ayudando a los usuarios a dominar rápidamente sus herramientas creativas. [1]</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>La sección 'Aprende' sugiere contenido educativo, y la función 'Arma tu PC' actúa como un tutorial guiado de construcción.</t>
+          <t>Las instrucciones son escasas y no siempre fáciles de encontrar, lo que dificulta el aprendizaje de nuevas funciones.</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Sería beneficioso incluir tutoriales de montaje o guías detalladas para principiantes, accesibles directamente desde las secciones 'Aprende' o 'Información'.</t>
+          <t>Crear tutoriales claros, accesibles y bien organizados, junto con un centro de ayuda intuitivo para usuarios.</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Overall User Experience</t>
+          <t>Conclusion</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Experiencia integral, pero puede ser abrumadora por la cantidad de funciones, aunque intuitiva en lo básico.</t>
+          <t>Una plataforma madura que equilibra comunicación personal con herramientas empresariales, manteniendo su relevancia global. [19]</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Muy atractiva y visual, intuitiva para compartir medios, pero puede generar sobrecarga de contenido visual.</t>
+          <t>Se consolidó como líder visual, evolucionando constantemente para satisfacer las demandas de creadores y usuarios. [5]</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Enfocada y eficiente para uso profesional, con rutas claras para networking y búsqueda de empleo, a veces algo formal.</t>
+          <t>Revolucionó el contenido de video corto, creando una cultura vibrante y una experiencia de usuario altamente adictiva. [1]</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Directa y funcional para encontrar componentes de PC, con un diseño limpio y sencillo para navegar fácilmente por los productos.</t>
+          <t>Este sitio ofrece una base sólida, pero con un potencial inmenso para mejorar su atractivo visual y funcionalidad. [6, 7]</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Para mejorar la experiencia general, optimizar los tiempos de carga de imágenes y añadir animaciones sutiles a las interacciones clave.</t>
+          <t>En general, el sitio podría beneficiarse enormemente de una renovación estética y funcional integral para destacar.</t>
         </is>
       </c>
     </row>

</xml_diff>